<commit_message>
data is classified, whether it includes conflict or not. Then that is parsed to the json and returned
</commit_message>
<xml_diff>
--- a/source/DEMO_FLIGHTPLAN.xlsx
+++ b/source/DEMO_FLIGHTPLAN.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Untitled/Hackathon2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerem/PyCharmProjects/manageFlights/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="620" windowWidth="27960" windowHeight="14040"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="14040"/>
   </bookViews>
   <sheets>
     <sheet name="XCREW.CREW_LEG_DEMO" sheetId="1" r:id="rId1"/>
@@ -1724,7 +1724,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1891,13 +1891,13 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
         <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Improvements for the readability and maintainability done.
</commit_message>
<xml_diff>
--- a/source/DEMO_FLIGHTPLAN.xlsx
+++ b/source/DEMO_FLIGHTPLAN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="14040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="XCREW.CREW_LEG_DEMO" sheetId="1" r:id="rId1"/>
@@ -1375,7 +1375,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1386,6 +1386,22 @@
     <font>
       <sz val="11"/>
       <name val="Dialog"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1405,8 +1421,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1417,7 +1435,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1722,7 +1742,7 @@
   </sheetPr>
   <dimension ref="A1:S626"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
@@ -1832,7 +1852,7 @@
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>443</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -38687,6 +38707,7 @@
   </sheetData>
   <autoFilter ref="A1:AE626"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>